<commit_message>
Insert sort + config file
</commit_message>
<xml_diff>
--- a/Traking.xlsx
+++ b/Traking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>№</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Shaker sort. Algorithms comparison</t>
+  </si>
+  <si>
+    <t>Insert sort</t>
+  </si>
+  <si>
+    <t>D:\Teaching\12.Algorithms\Tasks\Tasks</t>
   </si>
 </sst>
 </file>
@@ -619,7 +625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,11 +633,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" thickBottom="1"/>
@@ -1047,6 +1053,9 @@
       <c r="D27" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="E27" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="43.8" thickBot="1">
       <c r="A28" s="1">
@@ -1061,6 +1070,9 @@
       <c r="D28" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="E28" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="29" spans="1:5" thickBot="1">
       <c r="A29" s="1">
@@ -1072,6 +1084,9 @@
       <c r="C29" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E29" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="30" spans="1:5" thickBot="1">
       <c r="A30" s="1">
@@ -1082,6 +1097,23 @@
       </c>
       <c r="C30" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="E30" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" thickBot="1">
+      <c r="A31" s="1">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insert sort + config file (#54)
</commit_message>
<xml_diff>
--- a/Traking.xlsx
+++ b/Traking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>№</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Shaker sort. Algorithms comparison</t>
+  </si>
+  <si>
+    <t>Insert sort</t>
+  </si>
+  <si>
+    <t>D:\Teaching\12.Algorithms\Tasks\Tasks</t>
   </si>
 </sst>
 </file>
@@ -619,7 +625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,11 +633,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" thickBottom="1"/>
@@ -1047,6 +1053,9 @@
       <c r="D27" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="E27" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="43.8" thickBot="1">
       <c r="A28" s="1">
@@ -1061,6 +1070,9 @@
       <c r="D28" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="E28" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="29" spans="1:5" thickBot="1">
       <c r="A29" s="1">
@@ -1072,6 +1084,9 @@
       <c r="C29" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E29" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="30" spans="1:5" thickBot="1">
       <c r="A30" s="1">
@@ -1082,6 +1097,23 @@
       </c>
       <c r="C30" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="E30" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" thickBot="1">
+      <c r="A31" s="1">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>